<commit_message>
[AIOTAL-489] Added some of the validations
</commit_message>
<xml_diff>
--- a/src/assets/Sample Bulk Template.xlsx
+++ b/src/assets/Sample Bulk Template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adith_000\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adith_000\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,17 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>S.No</t>
   </si>
@@ -47,22 +42,33 @@
     <t>RPA Admin,Process Architect</t>
   </si>
   <si>
-    <t>gagana.puli@epsoftinc.com</t>
-  </si>
-  <si>
-    <t>Automation Designer,Process Analyst</t>
+    <t>aditya.jandhyala@epsoftinc.com</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>salma.shaik@epsoftinc.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -70,13 +76,7 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -99,25 +99,25 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -179,7 +179,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -214,7 +214,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -389,11 +389,6 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -402,68 +397,77 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="35.6640625" customWidth="1"/>
-    <col min="3" max="3" width="9" style="5"/>
+    <col min="3" max="3" width="9" style="1"/>
     <col min="4" max="4" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2" spans="1:4">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    <row r="3" spans="1:4">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="1"/>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" tooltip="mailto:lakshmi.kadali@epsoftinc.com"/>
     <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>